<commit_message>
commit final files for demo
</commit_message>
<xml_diff>
--- a/region.xlsx
+++ b/region.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\residences\directory-app2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CoyleMediaGroup\25f-cst8319-25f_cst8319_320_team-6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D902C1-7EAE-40E1-9344-988AC90C38C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F43C2BE-FD20-4C38-BD06-FFF4AB427ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="2232" windowWidth="12372" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="19935" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$5</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -405,37 +408,38 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A5" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>